<commit_message>
Added AUCratios to REGFLOW sheet
</commit_message>
<xml_diff>
--- a/UMRC6_HK2_UOK262_REGFLOW_summary.xlsx
+++ b/UMRC6_HK2_UOK262_REGFLOW_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D66A98B-4BAB-4781-8536-CD8203CF9861}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7C7F43-E097-451E-ADFB-7A2DAC5760F5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flux_fit_fixedT1" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="119">
   <si>
     <t>Date</t>
   </si>
@@ -449,6 +449,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -457,6 +458,7 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -465,16 +467,19 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -8355,16 +8360,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1253490</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>132080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>2540</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12416,14 +12421,14 @@
       <selection activeCell="U15" sqref="U15:V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.875" customWidth="1"/>
+    <col min="4" max="4" width="12.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.8984375" customWidth="1"/>
     <col min="19" max="19" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12445,7 +12450,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
@@ -12505,7 +12510,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>41555</v>
       </c>
@@ -12574,7 +12579,7 @@
         <v>1.9842115533333237E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>42</v>
       </c>
@@ -12643,7 +12648,7 @@
         <v>2.037861391190604E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>41754</v>
       </c>
@@ -12712,7 +12717,7 @@
         <v>9.6640555365881957E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>41754</v>
       </c>
@@ -12790,7 +12795,7 @@
         <v>1.6628261660609157E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>41754</v>
       </c>
@@ -12868,7 +12873,7 @@
         <v>6.0371419422555501E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>41810</v>
       </c>
@@ -12887,7 +12892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>41555</v>
       </c>
@@ -12912,7 +12917,7 @@
         <v>10.650537634408602</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="35"/>
       <c r="C10" s="18"/>
@@ -12920,12 +12925,12 @@
       <c r="E10" s="50"/>
       <c r="F10" s="21"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
         <v>41817</v>
       </c>
@@ -12994,7 +12999,7 @@
         <v>2.7830878357144356E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="17">
         <v>2</v>
@@ -13061,7 +13066,7 @@
         <v>3.5194916073554242E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>28</v>
       </c>
@@ -13094,7 +13099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="10">
         <v>3</v>
@@ -13176,7 +13181,7 @@
         <v>3.1512897215349297E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="10">
         <v>4</v>
@@ -13258,7 +13263,7 @@
         <v>1.8562816592332285E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>28</v>
       </c>
@@ -13287,12 +13292,12 @@
         <v>3.5981122470748465E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="16">
         <v>41817</v>
       </c>
@@ -13317,7 +13322,7 @@
         <v>3.2798911883276012</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="17">
         <v>2</v>
@@ -13344,7 +13349,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>80</v>
       </c>
@@ -13369,7 +13374,7 @@
         <v>2.0803566339902564</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
         <v>41817</v>
       </c>
@@ -13389,7 +13394,7 @@
         <v>96.319567076422288</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" s="16"/>
       <c r="B29" s="17">
         <v>2</v>
@@ -13407,7 +13412,7 @@
         <v>96.319567076422288</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
         <v>28</v>
       </c>
@@ -13427,7 +13432,7 @@
         <v>114.46925583409345</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
       <c r="B31" s="10">
         <v>3</v>
@@ -13445,7 +13450,7 @@
         <v>150.590870946183</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
       <c r="B32" s="10">
         <v>4</v>
@@ -13463,7 +13468,7 @@
         <v>150.5908709461826</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
         <v>28</v>
       </c>
@@ -13483,8 +13488,8 @@
         <v>82.11166839194307</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="57" t="s">
         <v>98</v>
       </c>
@@ -13498,7 +13503,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="62"/>
       <c r="B45" s="61"/>
       <c r="C45" s="61"/>
@@ -13508,7 +13513,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="62"/>
       <c r="B46" s="61" t="s">
         <v>73</v>
@@ -13519,7 +13524,7 @@
       <c r="D46" s="63"/>
       <c r="E46" s="61"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="64" t="s">
         <v>103</v>
       </c>
@@ -13534,7 +13539,7 @@
       </c>
       <c r="E47" s="65"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="62"/>
       <c r="B48" s="65" t="s">
         <v>55</v>
@@ -13547,7 +13552,7 @@
       </c>
       <c r="E48" s="65"/>
     </row>
-    <row r="49" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="68"/>
       <c r="B49" s="69" t="s">
         <v>52</v>
@@ -13560,7 +13565,7 @@
       </c>
       <c r="E49" s="65"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="72"/>
       <c r="B50" s="72"/>
       <c r="C50" s="72"/>
@@ -13592,13 +13597,13 @@
       <selection activeCell="H2" sqref="H2:T7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.875" customWidth="1"/>
+    <col min="4" max="4" width="12.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13617,7 +13622,7 @@
       <c r="Q1" s="82"/>
       <c r="R1" s="82"/>
     </row>
-    <row r="2" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
@@ -13671,7 +13676,7 @@
       <c r="S2" s="82"/>
       <c r="T2" s="75"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>41555</v>
       </c>
@@ -13732,7 +13737,7 @@
         <v>204203587.09977499</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>42</v>
       </c>
@@ -13787,7 +13792,7 @@
         <v>404280960.173729</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>41754</v>
       </c>
@@ -13842,7 +13847,7 @@
         <v>668450848.16999698</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>41754</v>
       </c>
@@ -13912,7 +13917,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>41754</v>
       </c>
@@ -13982,7 +13987,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>41810</v>
       </c>
@@ -14001,7 +14006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>41555</v>
       </c>
@@ -14026,7 +14031,7 @@
         <v>10.650537634408602</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="35"/>
       <c r="C10" s="18"/>
@@ -14034,12 +14039,12 @@
       <c r="E10" s="50"/>
       <c r="F10" s="21"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
         <v>41817</v>
       </c>
@@ -14097,7 +14102,7 @@
         <v>528480013.058981</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="17">
         <v>2</v>
@@ -14120,7 +14125,7 @@
         <v>5.1784713481947469</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>28</v>
       </c>
@@ -14145,7 +14150,7 @@
         <v>6.1542610663491102</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="10">
         <v>3</v>
@@ -14168,7 +14173,7 @@
         <v>8.096283384203387</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="10">
         <v>4</v>
@@ -14191,7 +14196,7 @@
         <v>8.0962833842033657</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>28</v>
       </c>
@@ -14216,12 +14221,12 @@
         <v>4.4146058275238209</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="16">
         <v>41817</v>
       </c>
@@ -14246,7 +14251,7 @@
         <v>3.2798911883276012</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="17">
         <v>2</v>
@@ -14273,7 +14278,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>80</v>
       </c>
@@ -14298,7 +14303,7 @@
         <v>2.0803566339902564</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
         <v>41817</v>
       </c>
@@ -14318,7 +14323,7 @@
         <v>96.319567076422288</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="16"/>
       <c r="B29" s="17">
         <v>2</v>
@@ -14336,7 +14341,7 @@
         <v>96.319567076422288</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
         <v>28</v>
       </c>
@@ -14356,7 +14361,7 @@
         <v>114.46925583409345</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
       <c r="B31" s="10">
         <v>3</v>
@@ -14374,7 +14379,7 @@
         <v>150.590870946183</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
       <c r="B32" s="10">
         <v>4</v>
@@ -14392,7 +14397,7 @@
         <v>150.5908709461826</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
         <v>28</v>
       </c>
@@ -14412,8 +14417,8 @@
         <v>82.11166839194307</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="57" t="s">
         <v>98</v>
       </c>
@@ -14427,7 +14432,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="62"/>
       <c r="B45" s="61"/>
       <c r="C45" s="61"/>
@@ -14437,7 +14442,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="62"/>
       <c r="B46" s="61" t="s">
         <v>73</v>
@@ -14448,7 +14453,7 @@
       <c r="D46" s="63"/>
       <c r="E46" s="61"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="64" t="s">
         <v>103</v>
       </c>
@@ -14463,7 +14468,7 @@
       </c>
       <c r="E47" s="65"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="62"/>
       <c r="B48" s="65" t="s">
         <v>55</v>
@@ -14476,7 +14481,7 @@
       </c>
       <c r="E48" s="65"/>
     </row>
-    <row r="49" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="68"/>
       <c r="B49" s="69" t="s">
         <v>52</v>
@@ -14489,7 +14494,7 @@
       </c>
       <c r="E49" s="65"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="72"/>
       <c r="B50" s="72"/>
       <c r="C50" s="72"/>
@@ -14518,34 +14523,34 @@
   <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E5" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="X11" sqref="X11"/>
+      <selection pane="bottomRight" activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="48" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.125" customWidth="1"/>
-    <col min="7" max="7" width="8.125" customWidth="1"/>
-    <col min="8" max="8" width="9.625" customWidth="1"/>
+    <col min="5" max="6" width="6.09765625" customWidth="1"/>
+    <col min="7" max="7" width="8.09765625" customWidth="1"/>
+    <col min="8" max="8" width="9.59765625" customWidth="1"/>
     <col min="9" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5" customWidth="1"/>
-    <col min="13" max="13" width="7.875" customWidth="1"/>
+    <col min="13" max="13" width="7.8984375" customWidth="1"/>
     <col min="14" max="14" width="9.5" customWidth="1"/>
     <col min="17" max="18" width="9.5" customWidth="1"/>
     <col min="19" max="20" width="6.5" customWidth="1"/>
-    <col min="21" max="21" width="6.125" customWidth="1"/>
-    <col min="22" max="22" width="8.625" customWidth="1"/>
-    <col min="23" max="23" width="7.375" customWidth="1"/>
-    <col min="24" max="24" width="7.875" customWidth="1"/>
+    <col min="21" max="21" width="6.09765625" customWidth="1"/>
+    <col min="22" max="22" width="8.59765625" customWidth="1"/>
+    <col min="23" max="23" width="7.3984375" customWidth="1"/>
+    <col min="24" max="24" width="7.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="42.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14598,7 +14603,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="1" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B2" s="26"/>
       <c r="C2" s="29" t="s">
         <v>6</v>
@@ -14652,7 +14657,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>41514</v>
       </c>
@@ -14731,7 +14736,7 @@
         <v>47.025074225724239</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>41544</v>
       </c>
@@ -14815,7 +14820,7 @@
         <v>56.019176476272349</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>41555</v>
       </c>
@@ -14893,7 +14898,7 @@
         <v>30.965555338033759</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>42</v>
       </c>
@@ -14968,7 +14973,7 @@
         <v>29.157233390543055</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>41558</v>
       </c>
@@ -15047,7 +15052,7 @@
         <v>39.247458596097573</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>41754</v>
       </c>
@@ -15125,7 +15130,7 @@
         <v>26.27676315391842</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>41555</v>
       </c>
@@ -15210,7 +15215,7 @@
         <v>21.955886789492045</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>42</v>
       </c>
@@ -15290,7 +15295,7 @@
         <v>20.308684949037882</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16">
         <v>41754</v>
       </c>
@@ -15372,7 +15377,7 @@
         <v>17.311036284635446</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="45"/>
       <c r="C12" s="46"/>
@@ -15393,12 +15398,12 @@
       <c r="W12" s="11"/>
       <c r="X12" s="11"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="O13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="O14" t="s">
         <v>19</v>
       </c>
@@ -15443,7 +15448,7 @@
         <v>38.115210196764899</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="P15">
         <f t="shared" ref="P15:W15" si="11">STDEV(P3,P4,P5,P6,P7,P8)/SQRT(COUNT(P3,P4,P5,P6,P7,P8))</f>
         <v>25.307494958104755</v>
@@ -15485,8 +15490,22 @@
         <v>4.735438780923201</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="15:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="13:26" x14ac:dyDescent="0.3">
+      <c r="M17">
+        <f>(M3+N3)/J3</f>
+        <v>2.4149060647788382E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="13:26" x14ac:dyDescent="0.3">
+      <c r="M18">
+        <f t="shared" ref="M18:M22" si="12">(M4+N4)/J4</f>
+        <v>1.5152452763920184E-2</v>
+      </c>
       <c r="O18" t="s">
         <v>46</v>
       </c>
@@ -15495,35 +15514,35 @@
         <v>148.65858216297462</v>
       </c>
       <c r="Q18">
-        <f t="shared" ref="Q18:X18" si="12">AVERAGE(Q9,Q10,Q11)</f>
+        <f t="shared" ref="Q18:X18" si="13">AVERAGE(Q9,Q10,Q11)</f>
         <v>1.6774991635859475E-5</v>
       </c>
       <c r="R18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.255737576721632E-6</v>
       </c>
       <c r="S18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.5678101893729037</v>
       </c>
       <c r="T18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.4209953270613689</v>
       </c>
       <c r="U18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.085083526388364</v>
       </c>
       <c r="V18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.1030729212581103E-5</v>
       </c>
       <c r="W18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6.9888055164342724</v>
       </c>
       <c r="X18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>163.73215889413032</v>
       </c>
       <c r="Y18">
@@ -15535,41 +15554,45 @@
         <v>19.858536007721792</v>
       </c>
     </row>
-    <row r="19" spans="15:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="13:26" x14ac:dyDescent="0.3">
+      <c r="M19">
+        <f t="shared" si="12"/>
+        <v>3.8341634647666607E-2</v>
+      </c>
       <c r="P19">
         <f>STDEV(P9,P10,P11)/SQRT(COUNT(P9,P10,P11))</f>
         <v>13.723691190131831</v>
       </c>
       <c r="Q19">
-        <f t="shared" ref="Q19:X19" si="13">STDEV(Q9,Q10,Q11)/SQRT(COUNT(Q9,Q10,Q11))</f>
+        <f t="shared" ref="Q19:X19" si="14">STDEV(Q9,Q10,Q11)/SQRT(COUNT(Q9,Q10,Q11))</f>
         <v>4.0797221893681171E-6</v>
       </c>
       <c r="R19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.1672105566140411E-6</v>
       </c>
       <c r="S19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.3894939706505944</v>
       </c>
       <c r="T19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.40325231509990844</v>
       </c>
       <c r="U19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.36185956914512996</v>
       </c>
       <c r="V19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5.2285486899228482E-6</v>
       </c>
       <c r="W19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.7876330947925514</v>
       </c>
       <c r="X19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.3137148000366552</v>
       </c>
       <c r="Y19">
@@ -15581,7 +15604,17 @@
         <v>1.3596120286246676</v>
       </c>
     </row>
-    <row r="21" spans="15:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="13:26" x14ac:dyDescent="0.3">
+      <c r="M20">
+        <f t="shared" si="12"/>
+        <v>2.068487453585803E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="13:26" x14ac:dyDescent="0.3">
+      <c r="M21">
+        <f t="shared" si="12"/>
+        <v>0.20650812254108958</v>
+      </c>
       <c r="O21" t="s">
         <v>47</v>
       </c>
@@ -15614,7 +15647,13 @@
         <v>8.1011056643610246E-2</v>
       </c>
     </row>
-    <row r="23" spans="15:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="13:26" x14ac:dyDescent="0.3">
+      <c r="M22">
+        <f t="shared" si="12"/>
+        <v>1.2015542328676536E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="13:26" x14ac:dyDescent="0.3">
       <c r="S23" t="s">
         <v>48</v>
       </c>
@@ -15654,25 +15693,25 @@
   <dimension ref="A1:Z31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="U3" sqref="U3:U5"/>
+      <selection pane="bottomRight" activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.125" customWidth="1"/>
-    <col min="6" max="7" width="7.375" customWidth="1"/>
-    <col min="8" max="8" width="8.125" customWidth="1"/>
-    <col min="9" max="9" width="9.625" customWidth="1"/>
+    <col min="2" max="2" width="5.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.09765625" customWidth="1"/>
+    <col min="6" max="7" width="7.3984375" customWidth="1"/>
+    <col min="8" max="8" width="8.09765625" customWidth="1"/>
+    <col min="9" max="9" width="9.59765625" customWidth="1"/>
     <col min="13" max="13" width="11.5" customWidth="1"/>
-    <col min="17" max="18" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15717,7 +15756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="1" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
@@ -15772,7 +15811,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>41817</v>
       </c>
@@ -15846,7 +15885,7 @@
         <v>26.466151363657506</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="17">
         <v>2</v>
@@ -15917,7 +15956,7 @@
         <v>15.037862493763953</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>28</v>
       </c>
@@ -15993,7 +16032,7 @@
         <v>28.128175507138195</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="10">
         <v>3</v>
@@ -16068,7 +16107,7 @@
         <v>30.214458136023481</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="10">
         <v>4</v>
@@ -16146,7 +16185,7 @@
         <v>35.049199837438806</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>28</v>
       </c>
@@ -16224,7 +16263,7 @@
         <v>21.169747393318278</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9"/>
       <c r="D9"/>
@@ -16241,7 +16280,7 @@
       <c r="V9"/>
       <c r="W9"/>
     </row>
-    <row r="10" spans="1:26" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10"/>
       <c r="D10"/>
@@ -16258,7 +16297,7 @@
       <c r="V10"/>
       <c r="W10"/>
     </row>
-    <row r="11" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20"/>
       <c r="O11" s="18" t="s">
         <v>29</v>
@@ -16304,7 +16343,7 @@
         <v>25.312191134132011</v>
       </c>
     </row>
-    <row r="12" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="17"/>
       <c r="P12" s="18" t="s">
         <v>31</v>
@@ -16342,12 +16381,12 @@
         <v>4.1145028424894114</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="11"/>
       <c r="N13" s="14"/>
     </row>
-    <row r="14" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="22"/>
       <c r="H14" s="23"/>
       <c r="L14" s="23"/>
@@ -16394,7 +16433,7 @@
         <v>28.811135122260186</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="D15" s="18"/>
@@ -16438,18 +16477,25 @@
         <v>4.0676277545136399</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="D16" s="15"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
+      <c r="M17">
+        <f>(M3+N3)/J3</f>
+        <v>3.2282790189882969E-2</v>
+      </c>
       <c r="P17" t="s">
         <v>47</v>
       </c>
@@ -16486,11 +16532,15 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
+      <c r="M18">
+        <f t="shared" ref="M18:M22" si="13">(M4+N4)/J4</f>
+        <v>1.9685042808742489E-2</v>
+      </c>
       <c r="Q18" s="21"/>
       <c r="R18" s="21"/>
       <c r="S18" s="21"/>
@@ -16499,30 +16549,46 @@
       <c r="V18" s="21"/>
       <c r="W18" s="21"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <f t="shared" si="13"/>
+        <v>6.0474682254895953E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B20" s="85"/>
       <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <f t="shared" si="13"/>
+        <v>3.9758174199751979E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="85"/>
       <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <f t="shared" si="13"/>
+        <v>4.4234246901484919E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B22" s="85"/>
       <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <f t="shared" si="13"/>
+        <v>3.9166027258272493E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="85"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="85"/>
       <c r="C24" s="2"/>
@@ -16534,7 +16600,7 @@
       <c r="J24" s="8"/>
       <c r="L24" s="7"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="85"/>
       <c r="C25" s="2"/>
@@ -16545,7 +16611,7 @@
       <c r="H25" s="7"/>
       <c r="L25" s="7"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B26" s="85"/>
       <c r="C26" s="2"/>
       <c r="D26" s="1"/>
@@ -16553,40 +16619,40 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B28" s="85"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="85"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B30" s="85"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="85"/>
       <c r="C31" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B20:B26"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="H1:O1"/>
     <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B20:B26"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -16607,22 +16673,22 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="M17" sqref="M17"/>
+      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.125" customWidth="1"/>
-    <col min="6" max="7" width="7.375" customWidth="1"/>
-    <col min="8" max="8" width="8.125" customWidth="1"/>
-    <col min="9" max="9" width="9.625" customWidth="1"/>
+    <col min="2" max="2" width="5.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.09765625" customWidth="1"/>
+    <col min="6" max="7" width="7.3984375" customWidth="1"/>
+    <col min="8" max="8" width="8.09765625" customWidth="1"/>
+    <col min="9" max="9" width="9.59765625" customWidth="1"/>
     <col min="13" max="13" width="11.5" customWidth="1"/>
-    <col min="17" max="17" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16667,7 +16733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" s="1" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
@@ -16722,7 +16788,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>41817</v>
       </c>
@@ -16796,7 +16862,7 @@
         <v>18.96424620586334</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="17">
         <v>2</v>
@@ -16867,7 +16933,7 @@
         <v>15.32589649665144</v>
       </c>
     </row>
-    <row r="5" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>80</v>
       </c>
@@ -16940,7 +17006,7 @@
         <v>17.861893157671531</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="10">
         <v>3</v>
@@ -17015,7 +17081,7 @@
         <v>12.831481870270606</v>
       </c>
     </row>
-    <row r="7" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="10">
         <v>4</v>
@@ -17086,7 +17152,7 @@
         <v>22.609357482598067</v>
       </c>
     </row>
-    <row r="8" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>81</v>
       </c>
@@ -17163,7 +17229,7 @@
         <v>15.094350887645922</v>
       </c>
     </row>
-    <row r="9" spans="1:25" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9"/>
       <c r="D9"/>
@@ -17180,7 +17246,7 @@
       <c r="V9"/>
       <c r="W9"/>
     </row>
-    <row r="10" spans="1:25" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10"/>
       <c r="D10"/>
@@ -17197,7 +17263,7 @@
       <c r="V10"/>
       <c r="W10"/>
     </row>
-    <row r="11" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="17"/>
       <c r="O11" s="18" t="s">
         <v>29</v>
@@ -17238,7 +17304,7 @@
         <v>17.384011953395436</v>
       </c>
     </row>
-    <row r="12" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="17"/>
       <c r="P12" s="18" t="s">
         <v>31</v>
@@ -17276,12 +17342,12 @@
         <v>1.0771374077743991</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="11"/>
       <c r="N13" s="14"/>
     </row>
-    <row r="14" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="22"/>
       <c r="H14" s="23"/>
       <c r="L14" s="23"/>
@@ -17328,7 +17394,7 @@
         <v>16.845063413504864</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="D15" s="18"/>
@@ -17372,7 +17438,7 @@
         <v>2.955247233520212</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="D16" s="15"/>
       <c r="E16" s="1"/>
@@ -17382,7 +17448,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -17423,7 +17489,7 @@
         <v>0.21548910391797854</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -17440,7 +17506,7 @@
       <c r="V18" s="21"/>
       <c r="W18" s="21"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="H19" s="5"/>
@@ -17449,7 +17515,7 @@
         <v>2.144050561350359E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B20" s="85"/>
       <c r="C20" s="24"/>
       <c r="M20">
@@ -17457,7 +17523,7 @@
         <v>1.9674636996941348E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="85"/>
       <c r="C21" s="24"/>
@@ -17466,7 +17532,7 @@
         <v>2.3050171114568169E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B22" s="85"/>
       <c r="C22" s="24"/>
       <c r="M22">
@@ -17474,12 +17540,12 @@
         <v>1.532183309869632E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="85"/>
       <c r="C23" s="24"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="85"/>
       <c r="C24" s="24"/>
@@ -17491,7 +17557,7 @@
       <c r="J24" s="8"/>
       <c r="L24" s="7"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="85"/>
       <c r="C25" s="24"/>
@@ -17502,7 +17568,7 @@
       <c r="H25" s="7"/>
       <c r="L25" s="7"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B26" s="85"/>
       <c r="C26" s="24"/>
       <c r="D26" s="1"/>
@@ -17510,23 +17576,23 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B28" s="85"/>
       <c r="C28" s="24"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="85"/>
       <c r="C29" s="24"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B30" s="85"/>
       <c r="C30" s="24"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="85"/>
       <c r="C31" s="24"/>
@@ -17564,9 +17630,9 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="78" t="s">
         <v>51</v>
       </c>
@@ -17597,7 +17663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="78"/>
       <c r="B2" s="79" t="s">
         <v>54</v>
@@ -17629,7 +17695,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="78" t="s">
         <v>52</v>
       </c>
@@ -17675,7 +17741,7 @@
         <v>38.115210196764899</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="78"/>
       <c r="B4" s="78" t="s">
         <v>32</v>
@@ -17720,7 +17786,7 @@
         <v>4.735438780923201</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="77"/>
       <c r="B5" s="77"/>
       <c r="C5" s="52"/>
@@ -17728,7 +17794,7 @@
       <c r="E5" s="52"/>
       <c r="F5" s="52"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="78" t="s">
         <v>55</v>
       </c>
@@ -17778,7 +17844,7 @@
         <v>23.210729788186551</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="78"/>
       <c r="B7" s="78" t="s">
         <v>32</v>
@@ -17827,7 +17893,7 @@
         <v>4.1145028424894114</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="77"/>
       <c r="B8" s="77"/>
       <c r="C8" s="52"/>
@@ -17835,7 +17901,7 @@
       <c r="E8" s="52"/>
       <c r="F8" s="52"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="78" t="s">
         <v>56</v>
       </c>
@@ -17885,7 +17951,7 @@
         <v>17.384011953395436</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="78"/>
       <c r="B10" s="78" t="s">
         <v>32</v>
@@ -17934,12 +18000,12 @@
         <v>1.0771374077743991</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B14" s="51" t="s">
         <v>57</v>
       </c>
@@ -17948,7 +18014,7 @@
       <c r="E14" s="83"/>
       <c r="F14" s="83"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="83"/>
@@ -17957,7 +18023,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -17999,7 +18065,7 @@
         <v>20.332449139125117</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>32</v>
       </c>
@@ -18038,7 +18104,7 @@
         <v>5.7699747711058071</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -18080,7 +18146,7 @@
         <v>26.396657864688702</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>32</v>
       </c>
@@ -18119,7 +18185,7 @@
         <v>4.1048825430274318</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -18161,7 +18227,7 @@
         <v>16.781229735095089</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>32</v>
       </c>
@@ -18202,16 +18268,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="80" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -18232,9 +18298,9 @@
       <selection activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>60</v>
       </c>
@@ -18272,7 +18338,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -18318,7 +18384,7 @@
         <v>1.0852095950154377</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -18350,7 +18416,7 @@
         <v>7.7766878108075754E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -18375,7 +18441,7 @@
         <v>13.750978835767379</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -18397,7 +18463,7 @@
         <v>0.43055668489574067</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -18410,7 +18476,7 @@
         <v>1.547935677291042</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -18427,7 +18493,7 @@
         <v>3.9391408698539805</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -18465,7 +18531,7 @@
         <v>2.8172389537523865E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -18478,7 +18544,7 @@
         <v>5.6498812608154232</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -18491,7 +18557,7 @@
         <v>2.5551541540482288</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -18522,7 +18588,7 @@
         <v>8.2869502840729242E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -18533,7 +18599,7 @@
         <v>5.5249037811164277</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -18544,12 +18610,12 @@
         <v>4.5985107019325584</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="51" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -18572,7 +18638,7 @@
         <v>1.3596120286246676</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -18587,7 +18653,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -18595,7 +18661,7 @@
         <v>17.311036284635446</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -18611,7 +18677,7 @@
         <v>4.0676277545136399</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -18619,7 +18685,7 @@
         <v>35.049199837438806</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -18627,7 +18693,7 @@
         <v>21.169747393318278</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -18650,7 +18716,7 @@
         <v>2.955247233520212</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -18658,7 +18724,7 @@
         <v>22.609357482598067</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -18687,9 +18753,9 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
         <v>87</v>
       </c>
@@ -18700,7 +18766,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>85</v>
       </c>
@@ -18712,7 +18778,7 @@
         <v>7.67</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -18745,7 +18811,7 @@
         <v>3.7638632635454153E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B4" s="16">
         <v>41514</v>
       </c>
@@ -18759,7 +18825,7 @@
         <v>7.81</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B5" s="16"/>
       <c r="C5">
         <v>3</v>
@@ -18785,7 +18851,7 @@
         <v>7.2280665813060185</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" s="16">
         <v>41544</v>
       </c>
@@ -18813,7 +18879,7 @@
         <v>6.8591980558930734</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" s="16">
         <v>41555</v>
       </c>
@@ -18841,7 +18907,7 @@
         <v>7.1179924242424244</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8" s="16"/>
       <c r="C8" t="s">
         <v>82</v>
@@ -18867,7 +18933,7 @@
         <v>7.124923857868021</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>42</v>
       </c>
@@ -18895,7 +18961,7 @@
         <v>7.049912935323384</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B10" s="16"/>
       <c r="C10" t="s">
         <v>82</v>
@@ -18921,7 +18987,7 @@
         <v>7.1887836107554426</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>41558</v>
       </c>
@@ -18946,7 +19012,7 @@
         <v>6.7032699167657546</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B12" s="16"/>
       <c r="C12" t="s">
         <v>82</v>
@@ -18972,7 +19038,7 @@
         <v>6.9363478260869558</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" s="16">
         <v>41754</v>
       </c>
@@ -19000,7 +19066,7 @@
         <v>6.6640983606557382</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>82</v>
       </c>
@@ -19028,7 +19094,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>30</v>
       </c>
@@ -19063,7 +19129,7 @@
         <v>7.3155793206654938</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>32</v>
       </c>
@@ -19098,7 +19164,7 @@
         <v>1.2644782225890234E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D17" s="50"/>
       <c r="E17" s="50"/>
       <c r="G17" s="50"/>
@@ -19107,7 +19173,7 @@
       <c r="K17" s="50"/>
       <c r="L17" s="50"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -19139,7 +19205,7 @@
       <c r="K18" s="50"/>
       <c r="L18" s="50"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>78</v>
       </c>
@@ -19165,7 +19231,7 @@
       <c r="K19" s="50"/>
       <c r="L19" s="50"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>79</v>
       </c>
@@ -19196,7 +19262,7 @@
       <c r="K20" s="50"/>
       <c r="L20" s="50"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>78</v>
       </c>
@@ -19226,7 +19292,7 @@
       <c r="K21" s="50"/>
       <c r="L21" s="50"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>30</v>
       </c>
@@ -19264,7 +19330,7 @@
         <v>7.329834230429749</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>32</v>
       </c>
@@ -19299,7 +19365,7 @@
         <v>3.8432991057540347E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D24" s="50"/>
       <c r="E24" s="50"/>
       <c r="G24" s="50"/>
@@ -19307,7 +19373,7 @@
       <c r="I24" s="50"/>
       <c r="K24" s="50"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -19330,7 +19396,7 @@
         <v>8.16</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>78</v>
       </c>
@@ -19347,7 +19413,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>79</v>
       </c>
@@ -19367,7 +19433,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>78</v>
       </c>
@@ -19384,7 +19450,7 @@
         <v>8.0500000000000007</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>30</v>
       </c>
@@ -19408,7 +19474,7 @@
         <v>7.6337499999999991</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
         <v>32</v>
       </c>
@@ -19447,7 +19513,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>